<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig-2@d49d19f9f2851a16cea64f377842ce84e7ec825e 🚀
</commit_message>
<xml_diff>
--- a/ValueSet-phenotypic-feature-assertion-vs.xlsx
+++ b/ValueSet-phenotypic-feature-assertion-vs.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Include #0" r:id="rId4" sheetId="2"/>
+    <sheet name="Include ValueSet #1" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +61,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-21T16:06:27+00:00</t>
+    <t>2025-07-22T19:44:39+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -96,16 +97,31 @@
     <t>BooleanType[null]</t>
   </si>
   <si>
-    <t>Codes</t>
-  </si>
-  <si>
-    <t>All codes</t>
+    <t>Concept</t>
+  </si>
+  <si>
+    <t>LA9633-4</t>
+  </si>
+  <si>
+    <t>Present</t>
+  </si>
+  <si>
+    <t>LA9634-2</t>
+  </si>
+  <si>
+    <t>Absent</t>
   </si>
   <si>
     <t>System URI</t>
   </si>
   <si>
-    <t>https://nih-ncpi.github.io/ncpi-fhir-ig-2/CodeSystem/phenotypic-feature-assertion</t>
+    <t>http://loinc.org</t>
+  </si>
+  <si>
+    <t>ValueSet URL</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/ValueSet/v3-NullFlavor</t>
   </si>
 </sst>
 </file>
@@ -372,7 +388,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -386,26 +402,67 @@
       <c r="A1" t="s" s="1">
         <v>27</v>
       </c>
+      <c r="B1" t="s" s="1">
+        <v>22</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
         <v>28</v>
       </c>
+      <c r="B2" t="s" s="2">
+        <v>29</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>30</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="30.703125" customWidth="true"/>
+    <col min="2" max="2" width="50.703125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>